<commit_message>
adding job and department in user import excell in progress
</commit_message>
<xml_diff>
--- a/projects/predyc-business/src/assets/files/plantilla carga estudiantes.xlsx
+++ b/projects/predyc-business/src/assets/files/plantilla carga estudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular\predyc-v3\projects\predyc-business\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo Prueba\Predyc\predyc-v3\projects\predyc-business\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9381C9EE-B346-49DE-A731-90C38226E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBF4B71-B47B-4D87-B07D-4B0150E6CC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2490" windowWidth="21600" windowHeight="11175" xr2:uid="{E71F9257-CAA0-456D-B242-C783B05093A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E71F9257-CAA0-456D-B242-C783B05093A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Teléfono</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Departamento</t>
   </si>
 </sst>
 </file>
@@ -398,21 +404,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C69F8B0-2B48-4285-B7E1-B84271F48646}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,6 +442,12 @@
       </c>
       <c r="G1" t="s">
         <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>